<commit_message>
Add test files and update lab 16
</commit_message>
<xml_diff>
--- a/manual/PipelineAnalysisTemplate.xlsx
+++ b/manual/PipelineAnalysisTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\potterst\Documents\CompOrg\Fall 2017\Day21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ELC3338\Fall2017\potter\ARM-Lab\manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12990"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="42">
   <si>
     <t>Fetch</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Write Back</t>
   </si>
   <si>
-    <t>zero</t>
-  </si>
-  <si>
     <t>npc_if</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>npc_ie</t>
   </si>
   <si>
-    <t>alu_result</t>
-  </si>
-  <si>
     <t>pc_src</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>alu_op_id</t>
   </si>
   <si>
-    <t>mem_write_id</t>
-  </si>
-  <si>
     <t>alu_src_id</t>
   </si>
   <si>
@@ -150,6 +141,15 @@
   </si>
   <si>
     <t>opcode_id</t>
+  </si>
+  <si>
+    <t>alu_result_ie</t>
+  </si>
+  <si>
+    <t>zero_ie</t>
+  </si>
+  <si>
+    <t>mem_write</t>
   </si>
 </sst>
 </file>
@@ -448,6 +448,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -463,10 +467,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,105 +778,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="21" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="21" t="s">
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="21" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="21" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="25"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="29"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="20"/>
@@ -894,7 +894,7 @@
         <v>3</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="2"/>
@@ -903,10 +903,10 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
@@ -917,10 +917,10 @@
       <c r="I4" s="14"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="1"/>
@@ -935,46 +935,46 @@
       <c r="A5" s="6"/>
       <c r="B5" s="1"/>
       <c r="C5" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="16" t="s">
+      <c r="M5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="17" t="s">
+      <c r="O5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>22</v>
       </c>
       <c r="Q5" s="6"/>
       <c r="R5" s="1"/>
@@ -985,16 +985,16 @@
       <c r="A6" s="6"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="8"/>
@@ -1016,78 +1016,78 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="29"/>
+      <c r="E7" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="24"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="29"/>
+      <c r="E8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="24"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="29"/>
+      <c r="E9" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="24"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -1115,10 +1115,10 @@
       <c r="E11" s="6"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="1"/>
@@ -1140,18 +1140,18 @@
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
+      <c r="G12" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
       <c r="O12" s="1"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="6"/>
@@ -1166,18 +1166,18 @@
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="28"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
+      <c r="G13" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
       <c r="O13" s="1"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="6"/>
@@ -1192,18 +1192,18 @@
       <c r="D14" s="8"/>
       <c r="E14" s="6"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="28"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
+      <c r="G14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
       <c r="O14" s="1"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="6"/>
@@ -1219,36 +1219,40 @@
       <c r="E15" s="6"/>
       <c r="F15" s="1"/>
       <c r="G15" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="L15" s="17"/>
+        <v>24</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="M15" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N15" s="16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O15" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="P15" s="17"/>
+        <v>25</v>
+      </c>
+      <c r="P15" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="Q15" s="16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R15" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="11"/>
@@ -1261,10 +1265,10 @@
       <c r="E16" s="6"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="1"/>
@@ -1286,18 +1290,22 @@
       <c r="D17" s="8"/>
       <c r="E17" s="6"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
+      <c r="G17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="14"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="O17" s="1"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="6"/>
@@ -1312,18 +1320,18 @@
       <c r="D18" s="8"/>
       <c r="E18" s="6"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="28"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="26"/>
+      <c r="G18" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="23"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="21"/>
       <c r="O18" s="1"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="6"/>
@@ -1338,18 +1346,18 @@
       <c r="D19" s="8"/>
       <c r="E19" s="6"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="26"/>
+      <c r="G19" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="21"/>
       <c r="O19" s="1"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="6"/>
@@ -1364,18 +1372,18 @@
       <c r="D20" s="8"/>
       <c r="E20" s="6"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
+      <c r="G20" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
       <c r="O20" s="1"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="6"/>
@@ -1390,18 +1398,18 @@
       <c r="D21" s="8"/>
       <c r="E21" s="6"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" s="28"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="26"/>
+      <c r="G21" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="21"/>
       <c r="O21" s="1"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="6"/>
@@ -1460,22 +1468,22 @@
       <c r="H24" s="8"/>
       <c r="I24" s="6"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="L24" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="M24" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="N24" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="O24" s="26"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
+      <c r="K24" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="N24" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="O24" s="21"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
       <c r="S24" s="1"/>
       <c r="T24" s="11"/>
     </row>
@@ -1491,16 +1499,16 @@
       <c r="I25" s="6"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="8"/>

</xml_diff>